<commit_message>
Ajusta parciais e layout do Pontos Corridos
</commit_message>
<xml_diff>
--- a/pontos_corridos/datasets_pontos_corridos/links_times_cartola_pontos_corridos.xlsx
+++ b/pontos_corridos/datasets_pontos_corridos/links_times_cartola_pontos_corridos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Nome do Time</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Link do Time</t>
   </si>
   <si>
+    <t>Arran Katoko FC</t>
+  </si>
+  <si>
     <t>bugredasmissões</t>
   </si>
   <si>
@@ -67,6 +70,9 @@
     <t>NHU PORÃ SAF.</t>
   </si>
   <si>
+    <t>Pepe Leal FC</t>
+  </si>
+  <si>
     <t>Pontaç0 F.C.</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t>Texas Club 2026</t>
   </si>
   <si>
+    <t>https://cartola.globo.com/#!/time/19833277</t>
+  </si>
+  <si>
     <t>https://cartola.globo.com/#!/time/19209079</t>
   </si>
   <si>
@@ -119,6 +128,9 @@
   </si>
   <si>
     <t>https://cartola.globo.com/#!/time/4088673</t>
+  </si>
+  <si>
+    <t>https://cartola.globo.com/#!/time/1326835</t>
   </si>
   <si>
     <t>https://cartola.globo.com/#!/time/20651178</t>
@@ -501,7 +513,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,10 +535,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>19209079</v>
+        <v>19833277</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -534,10 +546,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1488983</v>
+        <v>19209079</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -545,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>287965</v>
+        <v>1488983</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -556,10 +568,10 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>2916559</v>
+        <v>287965</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -567,10 +579,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>186283</v>
+        <v>2916559</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -578,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>2371918</v>
+        <v>186283</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -589,10 +601,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>16411206</v>
+        <v>2371918</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -600,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>14933455</v>
+        <v>16411206</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -611,10 +623,10 @@
         <v>11</v>
       </c>
       <c r="B10">
-        <v>47775950</v>
+        <v>14933455</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -622,10 +634,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>1747619</v>
+        <v>47775950</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -633,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>32966</v>
+        <v>1747619</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -644,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>44810918</v>
+        <v>32966</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -655,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>1867254</v>
+        <v>44810918</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -666,10 +678,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>4088673</v>
+        <v>1867254</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -677,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="B16">
-        <v>20651178</v>
+        <v>4088673</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -688,10 +700,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>14709358</v>
+        <v>1326835</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -699,10 +711,10 @@
         <v>19</v>
       </c>
       <c r="B18">
-        <v>184499</v>
+        <v>20651178</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -710,32 +722,56 @@
         <v>20</v>
       </c>
       <c r="B19">
+        <v>14709358</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>184499</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
         <v>1273719</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>38</v>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="!/time/19209079"/>
-    <hyperlink ref="C3" r:id="rId2" location="!/time/1488983"/>
-    <hyperlink ref="C4" r:id="rId3" location="!/time/287965"/>
-    <hyperlink ref="C5" r:id="rId4" location="!/time/2916559"/>
-    <hyperlink ref="C6" r:id="rId5" location="!/time/186283"/>
-    <hyperlink ref="C7" r:id="rId6" location="!/time/2371918"/>
-    <hyperlink ref="C8" r:id="rId7" location="!/time/16411206"/>
-    <hyperlink ref="C9" r:id="rId8" location="!/time/14933455"/>
-    <hyperlink ref="C10" r:id="rId9" location="!/time/47775950"/>
-    <hyperlink ref="C11" r:id="rId10" location="!/time/1747619"/>
-    <hyperlink ref="C12" r:id="rId11" location="!/time/32966"/>
-    <hyperlink ref="C13" r:id="rId12" location="!/time/44810918"/>
-    <hyperlink ref="C14" r:id="rId13" location="!/time/1867254"/>
-    <hyperlink ref="C15" r:id="rId14" location="!/time/4088673"/>
-    <hyperlink ref="C16" r:id="rId15" location="!/time/20651178"/>
-    <hyperlink ref="C17" r:id="rId16" location="!/time/14709358"/>
-    <hyperlink ref="C18" r:id="rId17" location="!/time/184499"/>
-    <hyperlink ref="C19" r:id="rId18" location="!/time/1273719"/>
+    <hyperlink ref="C2" r:id="rId1" location="!/time/19833277"/>
+    <hyperlink ref="C3" r:id="rId2" location="!/time/19209079"/>
+    <hyperlink ref="C4" r:id="rId3" location="!/time/1488983"/>
+    <hyperlink ref="C5" r:id="rId4" location="!/time/287965"/>
+    <hyperlink ref="C6" r:id="rId5" location="!/time/2916559"/>
+    <hyperlink ref="C7" r:id="rId6" location="!/time/186283"/>
+    <hyperlink ref="C8" r:id="rId7" location="!/time/2371918"/>
+    <hyperlink ref="C9" r:id="rId8" location="!/time/16411206"/>
+    <hyperlink ref="C10" r:id="rId9" location="!/time/14933455"/>
+    <hyperlink ref="C11" r:id="rId10" location="!/time/47775950"/>
+    <hyperlink ref="C12" r:id="rId11" location="!/time/1747619"/>
+    <hyperlink ref="C13" r:id="rId12" location="!/time/32966"/>
+    <hyperlink ref="C14" r:id="rId13" location="!/time/44810918"/>
+    <hyperlink ref="C15" r:id="rId14" location="!/time/1867254"/>
+    <hyperlink ref="C16" r:id="rId15" location="!/time/4088673"/>
+    <hyperlink ref="C17" r:id="rId16" location="!/time/1326835"/>
+    <hyperlink ref="C18" r:id="rId17" location="!/time/20651178"/>
+    <hyperlink ref="C19" r:id="rId18" location="!/time/14709358"/>
+    <hyperlink ref="C20" r:id="rId19" location="!/time/184499"/>
+    <hyperlink ref="C21" r:id="rId20" location="!/time/1273719"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>